<commit_message>
Tok med både en retning og begge retninger i Kostra 25 kollektivfelt
</commit_message>
<xml_diff>
--- a/kostraleveranse2020/Kostra 25 - Fylkesveg med kollektivfelt.xlsx
+++ b/kostraleveranse2020/Kostra 25 - Fylkesveg med kollektivfelt.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,6 +431,7 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="30"/>
     <col customWidth="1" max="2" min="2" width="30"/>
+    <col customWidth="1" max="3" min="3" width="30"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -441,7 +442,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Lengde kollektivfelt</t>
+          <t>Lengde en retning (m)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Lengde per kollektivfelt (m)</t>
         </is>
       </c>
     </row>
@@ -450,7 +456,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="n">
-        <v>31951.708</v>
+        <v>17786</v>
+      </c>
+      <c r="C2" t="n">
+        <v>31951</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +467,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>897.482</v>
+        <v>615</v>
+      </c>
+      <c r="C3" t="n">
+        <v>897</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +478,10 @@
         <v>30</v>
       </c>
       <c r="B4" t="n">
-        <v>9239.691000000001</v>
+        <v>8713</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9239</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +489,10 @@
         <v>34</v>
       </c>
       <c r="B5" t="n">
-        <v>741.986</v>
+        <v>370</v>
+      </c>
+      <c r="C5" t="n">
+        <v>741</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +500,10 @@
         <v>38</v>
       </c>
       <c r="B6" t="n">
-        <v>660.288</v>
+        <v>660</v>
+      </c>
+      <c r="C6" t="n">
+        <v>660</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +511,10 @@
         <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>2877.710999999999</v>
+        <v>2670</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2877</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +522,10 @@
         <v>46</v>
       </c>
       <c r="B8" t="n">
-        <v>10274.143</v>
+        <v>9160</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10274</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +533,10 @@
         <v>50</v>
       </c>
       <c r="B9" t="n">
-        <v>20459.26700000001</v>
+        <v>14937</v>
+      </c>
+      <c r="C9" t="n">
+        <v>20459</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +544,10 @@
         <v>54</v>
       </c>
       <c r="B10" t="n">
-        <v>1346.136</v>
+        <v>1302</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1346</v>
       </c>
     </row>
   </sheetData>
@@ -572,7 +605,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-02-05</t>
         </is>
       </c>
     </row>

</xml_diff>